<commit_message>
Update comparison data sheet
</commit_message>
<xml_diff>
--- a/CUDA_vs_OpenGL.xlsx
+++ b/CUDA_vs_OpenGL.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
   <si>
     <t>GPU:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,7 +98,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>~0</t>
+    <t>resolution: 512</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scene faces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bunny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>two cows</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dragon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all three</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rendering time (ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenGL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>With V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Without V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,39 +510,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="4.5" customHeight="1"/>
-    <row r="4" spans="1:7" hidden="1"/>
-    <row r="5" spans="1:7" hidden="1"/>
-    <row r="6" spans="1:7" ht="31.5" customHeight="1"/>
-    <row r="7" spans="1:7" ht="54" customHeight="1">
+    <row r="3" spans="1:16" ht="4.5" customHeight="1"/>
+    <row r="4" spans="1:16" hidden="1"/>
+    <row r="5" spans="1:16" hidden="1"/>
+    <row r="6" spans="1:16" ht="31.5" customHeight="1"/>
+    <row r="7" spans="1:16" ht="54" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="54" customHeight="1">
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="54" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="37.5" customHeight="1">
+    <row r="9" spans="1:16" ht="37.5" customHeight="1">
       <c r="D9" t="s">
         <v>7</v>
       </c>
@@ -506,7 +553,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:16">
       <c r="D10" t="s">
         <v>3</v>
       </c>
@@ -514,7 +561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -525,7 +572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -535,24 +582,71 @@
       <c r="G12">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="44.25" customHeight="1">
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="44.25" customHeight="1">
       <c r="D14" t="s">
         <v>8</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="J14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14">
+        <v>4968</v>
+      </c>
+      <c r="M14">
+        <v>31</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="D15" t="s">
         <v>3</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15">
+        <v>11608</v>
+      </c>
+      <c r="M15">
+        <v>16</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -562,8 +656,20 @@
       <c r="G16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="J16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16">
+        <v>100000</v>
+      </c>
+      <c r="M16">
+        <v>47</v>
+      </c>
+      <c r="P16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -573,25 +679,58 @@
       <c r="G17">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="45.75" customHeight="1"/>
-    <row r="19" spans="1:7" ht="33" customHeight="1">
+      <c r="J17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17">
+        <v>205804</v>
+      </c>
+      <c r="M17">
+        <v>55</v>
+      </c>
+      <c r="P17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="45.75" customHeight="1"/>
+    <row r="19" spans="1:16" ht="33" customHeight="1">
       <c r="D19" t="s">
         <v>10</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="J19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="D20" t="s">
         <v>3</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -601,8 +740,20 @@
       <c r="G21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="J21" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21">
+        <v>4968</v>
+      </c>
+      <c r="M21">
+        <v>109</v>
+      </c>
+      <c r="P21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -612,8 +763,48 @@
       <c r="G22">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="36.75" customHeight="1">
+      <c r="J22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22">
+        <v>11608</v>
+      </c>
+      <c r="M22">
+        <v>23</v>
+      </c>
+      <c r="P22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="J23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23">
+        <v>100000</v>
+      </c>
+      <c r="M23">
+        <v>156</v>
+      </c>
+      <c r="P23">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="J24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24">
+        <v>205804</v>
+      </c>
+      <c r="M24">
+        <v>141</v>
+      </c>
+      <c r="P24">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="36.75" customHeight="1">
       <c r="D25" t="s">
         <v>15</v>
       </c>
@@ -621,7 +812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:16">
       <c r="D26" t="s">
         <v>3</v>
       </c>
@@ -629,7 +820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -640,7 +831,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -651,14 +842,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:7" ht="39.75" customHeight="1">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:16" ht="39.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="32.25" customHeight="1">
+    <row r="32" spans="1:16" ht="32.25" customHeight="1">
       <c r="D32" t="s">
         <v>7</v>
       </c>
@@ -719,8 +910,8 @@
       <c r="D39">
         <v>23</v>
       </c>
-      <c r="G39" t="s">
-        <v>20</v>
+      <c r="G39">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:7">

</xml_diff>